<commit_message>
Linear Regression model built
</commit_message>
<xml_diff>
--- a/readonly/Data.xlsx
+++ b/readonly/Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1a1f1b61fa3318e9/Escritorio/Big Data/Project/Code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1a1f1b61fa3318e9/Escritorio/Big Data/Assignment/readonly/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{E7CE0AF9-6661-454F-8265-8EEEC3E4D81B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A6E4E1F3-2290-494E-BBF3-20926287B767}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{765569FA-3A4F-4B58-8D2E-94F718466B73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{22157CF9-CE82-4F5A-896D-178E6B3D2E8C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1C2F0FD3-906D-474B-9CE4-5BA0D60DF9DA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
   <si>
     <t>BOD(mg/L)</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -124,6 +124,168 @@
   <si>
     <t>Solar Radiation (MJ/m2)</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019/01/17</t>
+  </si>
+  <si>
+    <t>2019/02/21</t>
+  </si>
+  <si>
+    <t>2019/03/14</t>
+  </si>
+  <si>
+    <t>2019/03/21</t>
+  </si>
+  <si>
+    <t>2019/03/29</t>
+  </si>
+  <si>
+    <t>2019/04/04</t>
+  </si>
+  <si>
+    <t>2019/04/12</t>
+  </si>
+  <si>
+    <t>2019/04/18</t>
+  </si>
+  <si>
+    <t>2019/04/25</t>
+  </si>
+  <si>
+    <t>2019/05/09</t>
+  </si>
+  <si>
+    <t>2019/05/17</t>
+  </si>
+  <si>
+    <t>2019/05/23</t>
+  </si>
+  <si>
+    <t>2019/05/30</t>
+  </si>
+  <si>
+    <t>2019/06/05</t>
+  </si>
+  <si>
+    <t>2019/06/14</t>
+  </si>
+  <si>
+    <t>2019/06/20</t>
+  </si>
+  <si>
+    <t>2019/06/27</t>
+  </si>
+  <si>
+    <t>2019/07/04</t>
+  </si>
+  <si>
+    <t>2019/07/12</t>
+  </si>
+  <si>
+    <t>2019/07/18</t>
+  </si>
+  <si>
+    <t>2019/07/25</t>
+  </si>
+  <si>
+    <t>2019/07/31</t>
+  </si>
+  <si>
+    <t>2019/08/14</t>
+  </si>
+  <si>
+    <t>2019/08/22</t>
+  </si>
+  <si>
+    <t>2019/09/05</t>
+  </si>
+  <si>
+    <t>2019/09/19</t>
+  </si>
+  <si>
+    <t>2019/09/26</t>
+  </si>
+  <si>
+    <t>2019/10/04</t>
+  </si>
+  <si>
+    <t>2019/10/10</t>
+  </si>
+  <si>
+    <t>2019/10/17</t>
+  </si>
+  <si>
+    <t>2019/10/23</t>
+  </si>
+  <si>
+    <t>2019/10/31</t>
+  </si>
+  <si>
+    <t>2019/11/06</t>
+  </si>
+  <si>
+    <t>2019/11/14</t>
+  </si>
+  <si>
+    <t>2019/11/20</t>
+  </si>
+  <si>
+    <t>2019/11/28</t>
+  </si>
+  <si>
+    <t>2019/12/05</t>
+  </si>
+  <si>
+    <t>2020/01/16</t>
+  </si>
+  <si>
+    <t>2020/02/20</t>
+  </si>
+  <si>
+    <t>2020/08/21</t>
+  </si>
+  <si>
+    <t>2020/08/27</t>
+  </si>
+  <si>
+    <t>2020/09/03</t>
+  </si>
+  <si>
+    <t>2020/09/10</t>
+  </si>
+  <si>
+    <t>2020/09/18</t>
+  </si>
+  <si>
+    <t>2020/09/24</t>
+  </si>
+  <si>
+    <t>2020/10/08</t>
+  </si>
+  <si>
+    <t>2020/10/15</t>
+  </si>
+  <si>
+    <t>2020/10/23</t>
+  </si>
+  <si>
+    <t>2020/10/29</t>
+  </si>
+  <si>
+    <t>2020/11/05</t>
+  </si>
+  <si>
+    <t>2020/11/12</t>
+  </si>
+  <si>
+    <t>2020/11/20</t>
+  </si>
+  <si>
+    <t>2020/11/26</t>
+  </si>
+  <si>
+    <t>2020/12/10</t>
   </si>
 </sst>
 </file>
@@ -175,11 +337,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -496,19 +657,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{231183D9-3A79-4FCB-8FF5-32C53B6754FD}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -532,444 +693,1524 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16.5">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="C2">
+        <v>-0.3</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>1013.4</v>
+      </c>
+      <c r="F2">
+        <v>11.07</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="1">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>2.4</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>1015.9</v>
+      </c>
+      <c r="F3">
+        <v>14.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>1011.9</v>
+      </c>
+      <c r="F4">
+        <v>14.02</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="1">
+        <v>10.5</v>
+      </c>
+      <c r="C5">
+        <v>7.1</v>
+      </c>
+      <c r="D5">
+        <v>3.3</v>
+      </c>
+      <c r="E5">
+        <v>998.1</v>
+      </c>
+      <c r="F5">
+        <v>7.51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="1">
+        <v>6.1</v>
+      </c>
+      <c r="C6">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>1003.5</v>
+      </c>
+      <c r="F6">
+        <v>21.22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="C7">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>1007.2</v>
+      </c>
+      <c r="F7">
+        <v>22.72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="1">
+        <v>3.7</v>
+      </c>
+      <c r="C8">
+        <v>11.4</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>1007.7</v>
+      </c>
+      <c r="F8">
+        <v>23.73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="1">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>12.6</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>1001.8</v>
+      </c>
+      <c r="F9">
+        <v>5.88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="1">
+        <v>7.7</v>
+      </c>
+      <c r="C10">
+        <v>13.2</v>
+      </c>
+      <c r="D10">
+        <v>11.3</v>
+      </c>
+      <c r="E10">
+        <v>996.9</v>
+      </c>
+      <c r="F10">
+        <v>3.48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="1">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>1000.8</v>
+      </c>
+      <c r="F11">
+        <v>25.46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="1">
+        <v>4.3</v>
+      </c>
+      <c r="C12">
+        <v>23.6</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>1002.2</v>
+      </c>
+      <c r="F12">
+        <v>14.72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="C13">
+        <v>22.1</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>998.4</v>
+      </c>
+      <c r="F13">
+        <v>27.36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="1">
+        <v>5.3</v>
+      </c>
+      <c r="C14">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>1000.7</v>
+      </c>
+      <c r="F14">
+        <v>18.28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C15">
+        <v>23</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>1001.8</v>
+      </c>
+      <c r="F15">
+        <v>24.14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="C16">
+        <v>23</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>995.3</v>
+      </c>
+      <c r="F16">
+        <v>19.46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C17">
+        <v>22.7</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>997.1</v>
+      </c>
+      <c r="F17">
+        <v>20.91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="1">
+        <v>3.7</v>
+      </c>
+      <c r="C18">
+        <v>25.5</v>
+      </c>
+      <c r="D18">
+        <v>1.4</v>
+      </c>
+      <c r="E18">
+        <v>990.9</v>
+      </c>
+      <c r="F18">
+        <v>14.79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="C19">
+        <v>25.4</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>996.5</v>
+      </c>
+      <c r="F19">
+        <v>27.41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="C20">
+        <v>23.6</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>996.3</v>
+      </c>
+      <c r="F20">
+        <v>18.43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C21">
+        <v>26.9</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>998.7</v>
+      </c>
+      <c r="F21">
+        <v>12.78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="1">
+        <v>8.6</v>
+      </c>
+      <c r="C22">
+        <v>26.3</v>
+      </c>
+      <c r="D22">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="E22">
+        <v>994.6</v>
+      </c>
+      <c r="F22">
+        <v>3.47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="1">
+        <v>6.2</v>
+      </c>
+      <c r="C23">
+        <v>25.8</v>
+      </c>
+      <c r="D23">
+        <v>62.3</v>
+      </c>
+      <c r="E23">
+        <v>999.3</v>
+      </c>
+      <c r="F23">
+        <v>3.01</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C24">
+        <v>30.4</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>990.2</v>
+      </c>
+      <c r="F24">
+        <v>20.99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="1">
+        <v>3.8</v>
+      </c>
+      <c r="C25">
+        <v>26.9</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>996.5</v>
+      </c>
+      <c r="F25">
+        <v>23.16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="1">
+        <v>6.6</v>
+      </c>
+      <c r="C26">
+        <v>23</v>
+      </c>
+      <c r="D26">
+        <v>36.4</v>
+      </c>
+      <c r="E26">
+        <v>1001.9</v>
+      </c>
+      <c r="F26">
+        <v>6.07</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="C27">
+        <v>19.5</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>1008.2</v>
+      </c>
+      <c r="F27">
+        <v>19.829999999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="C28">
+        <v>22.9</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>1013.6</v>
+      </c>
+      <c r="F28">
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="C29">
+        <v>22.4</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>1002.4</v>
+      </c>
+      <c r="F29">
+        <v>16.23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="C30">
+        <v>15.2</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>1006.3</v>
+      </c>
+      <c r="F30">
+        <v>8.06</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="C31">
+        <v>15.4</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>1014.1</v>
+      </c>
+      <c r="F31">
+        <v>12.02</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="C32">
+        <v>17</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>1008.9</v>
+      </c>
+      <c r="F32">
+        <v>8.08</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="C33">
+        <v>14.8</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>1010.1</v>
+      </c>
+      <c r="F33">
+        <v>10.34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="C34">
+        <v>11</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>1006.6</v>
+      </c>
+      <c r="F34">
+        <v>10.63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B35" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="C35">
+        <v>1.3</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>1013.7</v>
+      </c>
+      <c r="F35">
+        <v>13.15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B36" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="C36">
+        <v>0.5</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>1020.9</v>
+      </c>
+      <c r="F36">
+        <v>12.18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B37" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="C37">
+        <v>3.5</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>1019.1</v>
+      </c>
+      <c r="F37">
+        <v>11.21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B38" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="C38">
+        <v>-4.4000000000000004</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>1025.3</v>
+      </c>
+      <c r="F38">
+        <v>11.34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" s="1">
+        <v>1.7</v>
+      </c>
+      <c r="C39">
+        <v>-1.7</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>1016.3</v>
+      </c>
+      <c r="F39">
+        <v>10.75</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B40" s="1">
+        <v>5.8</v>
+      </c>
+      <c r="C40">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>1022.6</v>
+      </c>
+      <c r="F40">
+        <v>13.71</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B41" s="1">
         <v>3.4</v>
       </c>
-      <c r="C2">
+      <c r="C41">
         <v>1.4</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
         <v>1014.5</v>
       </c>
-      <c r="F2">
+      <c r="F41">
         <v>19.25</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16.5">
-      <c r="A3" s="2" t="s">
+    <row r="42" spans="1:6">
+      <c r="A42" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B42" s="1">
         <v>2.6</v>
       </c>
-      <c r="C3">
+      <c r="C42">
         <v>6.8</v>
       </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
         <v>1010.9</v>
       </c>
-      <c r="F3">
+      <c r="F42">
         <v>14.32</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16.5">
-      <c r="A4" s="2" t="s">
+    <row r="43" spans="1:6">
+      <c r="A43" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B43" s="1">
         <v>3.8</v>
       </c>
-      <c r="C4">
+      <c r="C43">
         <v>8.8000000000000007</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
         <v>1003.3</v>
       </c>
-      <c r="F4">
+      <c r="F43">
         <v>20.58</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16.5">
-      <c r="A5" s="2" t="s">
+    <row r="44" spans="1:6">
+      <c r="A44" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B44" s="1">
         <v>4</v>
       </c>
-      <c r="C5">
+      <c r="C44">
         <v>11.9</v>
       </c>
-      <c r="D5">
+      <c r="D44">
         <v>2</v>
       </c>
-      <c r="E5">
+      <c r="E44">
         <v>1003.2</v>
       </c>
-      <c r="F5">
+      <c r="F44">
         <v>17.04</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16.5">
-      <c r="A6" s="2" t="s">
+    <row r="45" spans="1:6">
+      <c r="A45" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B45" s="1">
         <v>2.4</v>
       </c>
-      <c r="C6">
+      <c r="C45">
         <v>10</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
         <v>1010.5</v>
       </c>
-      <c r="F6">
+      <c r="F45">
         <v>22.56</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16.5">
-      <c r="A7" s="2" t="s">
+    <row r="46" spans="1:6">
+      <c r="A46" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B46" s="1">
         <v>3.1</v>
       </c>
-      <c r="C7">
+      <c r="C46">
         <v>8.9</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
         <v>1011.5</v>
       </c>
-      <c r="F7">
+      <c r="F46">
         <v>24.79</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16.5">
-      <c r="A8" s="2" t="s">
+    <row r="47" spans="1:6">
+      <c r="A47" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B47" s="1">
         <v>2.7</v>
       </c>
-      <c r="C8">
+      <c r="C47">
         <v>16</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
         <v>1006.1</v>
       </c>
-      <c r="F8">
+      <c r="F47">
         <v>22.96</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16.5">
-      <c r="A9" s="2" t="s">
+    <row r="48" spans="1:6">
+      <c r="A48" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B48" s="1">
         <v>3</v>
       </c>
-      <c r="C9">
+      <c r="C48">
         <v>7.9</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
         <v>1005.6</v>
       </c>
-      <c r="F9">
+      <c r="F48">
         <v>25.72</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16.5">
-      <c r="A10" s="2" t="s">
+    <row r="49" spans="1:6">
+      <c r="A49" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B49" s="1">
         <v>3.2</v>
       </c>
-      <c r="C10">
+      <c r="C49">
         <v>14.9</v>
       </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
         <v>1009</v>
       </c>
-      <c r="F10">
+      <c r="F49">
         <v>26.1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16.5">
-      <c r="A11" s="2" t="s">
+    <row r="50" spans="1:6">
+      <c r="A50" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B50" s="1">
         <v>2.9</v>
       </c>
-      <c r="C11">
+      <c r="C50">
         <v>19.899999999999999</v>
       </c>
-      <c r="D11">
+      <c r="D50">
         <v>2.2999999999999998</v>
       </c>
-      <c r="E11">
+      <c r="E50">
         <v>1004.4</v>
       </c>
-      <c r="F11">
+      <c r="F50">
         <v>23.26</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="16.5">
-      <c r="A12" s="2" t="s">
+    <row r="51" spans="1:6">
+      <c r="A51" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B51" s="1">
         <v>2.5</v>
       </c>
-      <c r="C12">
+      <c r="C51">
         <v>19.3</v>
       </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
         <v>1006</v>
       </c>
-      <c r="F12">
+      <c r="F51">
         <v>20.64</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="16.5">
-      <c r="A13" s="2" t="s">
+    <row r="52" spans="1:6">
+      <c r="A52" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B52" s="1">
         <v>2.7</v>
       </c>
-      <c r="C13">
+      <c r="C52">
         <v>17.399999999999999</v>
       </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
         <v>1004.4</v>
       </c>
-      <c r="F13">
+      <c r="F52">
         <v>24.35</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="16.5">
-      <c r="A14" s="2" t="s">
+    <row r="53" spans="1:6">
+      <c r="A53" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B53" s="1">
         <v>2.5</v>
       </c>
-      <c r="C14">
+      <c r="C53">
         <v>18.7</v>
       </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
         <v>999.6</v>
       </c>
-      <c r="F14">
+      <c r="F53">
         <v>22.83</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="16.5">
-      <c r="A15" s="2" t="s">
+    <row r="54" spans="1:6">
+      <c r="A54" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B54" s="1">
         <v>3.2</v>
       </c>
-      <c r="C15">
+      <c r="C54">
         <v>21.9</v>
       </c>
-      <c r="D15">
+      <c r="D54">
         <v>0.2</v>
       </c>
-      <c r="E15">
+      <c r="E54">
         <v>994.1</v>
       </c>
-      <c r="F15">
+      <c r="F54">
         <v>19.77</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="16.5">
-      <c r="A16" s="2" t="s">
+    <row r="55" spans="1:6">
+      <c r="A55" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B55" s="1">
         <v>5.8</v>
       </c>
-      <c r="C16">
+      <c r="C55">
         <v>26.1</v>
       </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
         <v>993.7</v>
       </c>
-      <c r="F16">
+      <c r="F55">
         <v>26.03</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="16.5">
-      <c r="A17" s="2" t="s">
+    <row r="56" spans="1:6">
+      <c r="A56" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B56" s="1">
         <v>4.7</v>
       </c>
-      <c r="C17">
+      <c r="C56">
         <v>24.7</v>
       </c>
-      <c r="D17">
+      <c r="D56">
         <v>0.1</v>
       </c>
-      <c r="E17">
+      <c r="E56">
         <v>996.4</v>
       </c>
-      <c r="F17">
+      <c r="F56">
         <v>19.600000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="16.5">
-      <c r="A18" s="2" t="s">
+    <row r="57" spans="1:6">
+      <c r="A57" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B57" s="1">
         <v>12</v>
       </c>
-      <c r="C18">
+      <c r="C57">
         <v>21.6</v>
       </c>
-      <c r="D18">
+      <c r="D57">
         <v>13.3</v>
       </c>
-      <c r="E18">
+      <c r="E57">
         <v>991.8</v>
       </c>
-      <c r="F18">
+      <c r="F57">
         <v>6.11</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="16.5">
-      <c r="A19" s="2" t="s">
+    <row r="58" spans="1:6">
+      <c r="A58" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B58" s="1">
         <v>1.8</v>
       </c>
-      <c r="C19">
+      <c r="C58">
         <v>25.5</v>
       </c>
-      <c r="D19">
+      <c r="D58">
         <v>0.1</v>
       </c>
-      <c r="E19">
+      <c r="E58">
         <v>1000.5</v>
       </c>
-      <c r="F19">
+      <c r="F58">
         <v>27.47</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="16.5">
-      <c r="A20" s="2" t="s">
+    <row r="59" spans="1:6">
+      <c r="A59" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B59" s="1">
         <v>2</v>
       </c>
-      <c r="C20">
+      <c r="C59">
         <v>27.5</v>
       </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59">
         <v>994</v>
       </c>
-      <c r="F20">
+      <c r="F59">
         <v>23.1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="16.5">
-      <c r="A21" s="2" t="s">
+    <row r="60" spans="1:6">
+      <c r="A60" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B60" s="1">
         <v>1.9</v>
       </c>
-      <c r="C21">
+      <c r="C60">
         <v>25</v>
       </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60">
         <v>997</v>
       </c>
-      <c r="F21">
+      <c r="F60">
         <v>25.76</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="16.5">
-      <c r="A22" s="2" t="s">
+    <row r="61" spans="1:6">
+      <c r="A61" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B61" s="1">
         <v>4.5</v>
       </c>
-      <c r="C22">
+      <c r="C61">
         <v>21.1</v>
       </c>
-      <c r="D22">
+      <c r="D61">
         <v>103.1</v>
       </c>
-      <c r="E22">
+      <c r="E61">
         <v>995.7</v>
       </c>
-      <c r="F22">
+      <c r="F61">
         <v>2.72</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="16.5">
-      <c r="A23" s="2" t="s">
+    <row r="62" spans="1:6">
+      <c r="A62" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B62" s="1">
         <v>9.6999999999999993</v>
       </c>
-      <c r="C23">
+      <c r="C62">
         <v>25.3</v>
       </c>
-      <c r="D23">
+      <c r="D62">
         <v>0.1</v>
       </c>
-      <c r="E23">
+      <c r="E62">
         <v>1003.4</v>
       </c>
-      <c r="F23">
+      <c r="F62">
         <v>15.34</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B63" s="1">
+        <v>11.9</v>
+      </c>
+      <c r="C63">
+        <v>26.6</v>
+      </c>
+      <c r="D63">
+        <v>2.5</v>
+      </c>
+      <c r="E63">
+        <v>1003.9</v>
+      </c>
+      <c r="F63">
+        <v>8.74</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B64" s="1">
+        <v>5.9</v>
+      </c>
+      <c r="C64">
+        <v>27.1</v>
+      </c>
+      <c r="D64">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="E64">
+        <v>991.3</v>
+      </c>
+      <c r="F64">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B65" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="C65">
+        <v>22.7</v>
+      </c>
+      <c r="D65">
+        <v>29.8</v>
+      </c>
+      <c r="E65">
+        <v>987.3</v>
+      </c>
+      <c r="F65">
+        <v>13.51</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B66" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="C66">
+        <v>22.8</v>
+      </c>
+      <c r="D66">
+        <v>3.9</v>
+      </c>
+      <c r="E66">
+        <v>999.1</v>
+      </c>
+      <c r="F66">
+        <v>19.170000000000002</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B67" s="1">
+        <v>4</v>
+      </c>
+      <c r="C67">
+        <v>21.5</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>1002.7</v>
+      </c>
+      <c r="F67">
+        <v>21.24</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B68" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C68">
+        <v>20.6</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="E68">
+        <v>1005.3</v>
+      </c>
+      <c r="F68">
+        <v>18.54</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B69" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="C69">
+        <v>17.2</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="E69">
+        <v>1016.7</v>
+      </c>
+      <c r="F69">
+        <v>19.27</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B70" s="1">
+        <v>1.7</v>
+      </c>
+      <c r="C70">
+        <v>11.7</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70">
+        <v>1015.8</v>
+      </c>
+      <c r="F70">
+        <v>14.48</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B71" s="1">
+        <v>1.7</v>
+      </c>
+      <c r="C71">
+        <v>8.6</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>1004.9</v>
+      </c>
+      <c r="F71">
+        <v>17.010000000000002</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B72" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="C72">
+        <v>10.8</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72">
+        <v>1013.7</v>
+      </c>
+      <c r="F72">
+        <v>13.77</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B73" s="1">
+        <v>1.9</v>
+      </c>
+      <c r="C73">
+        <v>9.6</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <v>1016.7</v>
+      </c>
+      <c r="F73">
+        <v>12.77</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B74" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="C74">
+        <v>10.4</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="E74">
+        <v>1019.9</v>
+      </c>
+      <c r="F74">
+        <v>12.27</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B75" s="1">
+        <v>5.7</v>
+      </c>
+      <c r="C75">
+        <v>2.8</v>
+      </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
+      <c r="E75">
+        <v>1009.3</v>
+      </c>
+      <c r="F75">
+        <v>2.74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B76" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="C76">
+        <v>5.6</v>
+      </c>
+      <c r="D76">
+        <v>0</v>
+      </c>
+      <c r="E76">
+        <v>1016.5</v>
+      </c>
+      <c r="F76">
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B77" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="C77">
+        <v>5.8</v>
+      </c>
+      <c r="D77">
+        <v>0</v>
+      </c>
+      <c r="E77">
+        <v>1011.8</v>
+      </c>
+      <c r="F77">
+        <v>4.74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>